<commit_message>
Path changes for Toolik test and "single season" ToolikTest csv file created.
</commit_message>
<xml_diff>
--- a/ToolikLake/ParameterInputsToolik.xlsx
+++ b/ToolikLake/ParameterInputsToolik.xlsx
@@ -456,7 +456,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +530,9 @@
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>2.9</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -539,7 +541,9 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>